<commit_message>
Add soft deletion functionlity in visa expense and visa installment and also change the ledger interface
</commit_message>
<xml_diff>
--- a/public/sample/rider_voucher_sample.xlsx
+++ b/public/sample/rider_voucher_sample.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jutt computer\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xammp1\htdocs\erpbk\public\sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="15">
   <si>
     <t>Billing Month</t>
   </si>
@@ -59,16 +59,19 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Penalty Voucher</t>
+    <t>Vendor Charges Voucher</t>
   </si>
   <si>
-    <t>Incentive Voucher</t>
+    <t>Incentive</t>
   </si>
   <si>
-    <t>COD Voucher</t>
+    <t>Penalty</t>
   </si>
   <si>
-    <t>Vendor Charges Voucher</t>
+    <t>COD</t>
+  </si>
+  <si>
+    <t>Advance Loan</t>
   </si>
 </sst>
 </file>
@@ -452,7 +455,7 @@
   <dimension ref="A1:G328"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -525,7 +528,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F3" t="s">
         <v>9</v>
@@ -571,7 +574,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F5" t="s">
         <v>9</v>
@@ -594,7 +597,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F6" t="s">
         <v>9</v>
@@ -604,9 +607,27 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="2"/>
-      <c r="G7" s="4"/>
+      <c r="A7" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="3">
+        <v>45976</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>

</xml_diff>